<commit_message>
History and custom implementation
</commit_message>
<xml_diff>
--- a/resources/Repository Setup.xlsx
+++ b/resources/Repository Setup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="14565" windowHeight="7245" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="14565" windowHeight="7245" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8283" uniqueCount="2721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8345" uniqueCount="2734">
   <si>
     <t>identifier</t>
   </si>
@@ -8433,6 +8433,45 @@
   </si>
   <si>
     <t>Après création</t>
+  </si>
+  <si>
+    <t>Quotes</t>
+  </si>
+  <si>
+    <t>Valorisations</t>
+  </si>
+  <si>
+    <t>Input an application date</t>
+  </si>
+  <si>
+    <t>Saisir une date d'application</t>
+  </si>
+  <si>
+    <t>Input a numerical value</t>
+  </si>
+  <si>
+    <t>Saisir un nombre</t>
+  </si>
+  <si>
+    <t>Date.placeholder</t>
+  </si>
+  <si>
+    <t>Value.placeholder</t>
+  </si>
+  <si>
+    <t>global.reset_custom</t>
+  </si>
+  <si>
+    <t>Reset custom information</t>
+  </si>
+  <si>
+    <t>Reset custom</t>
+  </si>
+  <si>
+    <t>Réinitialiser les données personnalisées</t>
+  </si>
+  <si>
+    <t>reset_custom_information</t>
   </si>
 </sst>
 </file>
@@ -9270,8 +9309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E658"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:A49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21004,10 +21043,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21324,6 +21363,52 @@
       </c>
       <c r="H13" s="5" t="s">
         <v>2519</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>2729</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>2733</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>2730</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>2731</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>1762</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>2729</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>2733</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>2730</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>2731</v>
       </c>
     </row>
   </sheetData>
@@ -21581,10 +21666,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1791"/>
+  <dimension ref="A1:E1807"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1731" workbookViewId="0">
-      <selection activeCell="C1754" sqref="C1754"/>
+    <sheetView topLeftCell="A1795" workbookViewId="0">
+      <selection activeCell="C1807" sqref="C1807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42599,6 +42684,182 @@
         <v>2711</v>
       </c>
     </row>
+    <row r="1792" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1792" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B1792" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1792" t="s">
+        <v>2721</v>
+      </c>
+    </row>
+    <row r="1793" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1793" t="s">
+        <v>2721</v>
+      </c>
+      <c r="B1793" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1793" t="s">
+        <v>2722</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1794" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B1794" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1794" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1795" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B1795" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1795" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1796" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B1796" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1796" t="s">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1797" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B1797" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1797" t="s">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1798" s="5" t="s">
+        <v>1640</v>
+      </c>
+      <c r="B1798" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1798" t="s">
+        <v>1640</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1799" s="5" t="s">
+        <v>1705</v>
+      </c>
+      <c r="B1799" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1799" t="s">
+        <v>1705</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1800" s="5" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B1800" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1800" t="s">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1801" s="5" t="s">
+        <v>2700</v>
+      </c>
+      <c r="B1801" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1801" t="s">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1802" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B1802" s="5" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1802" t="s">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1803" t="s">
+        <v>2727</v>
+      </c>
+      <c r="B1803" s="5" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1803" t="s">
+        <v>2724</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1804" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B1804" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1804" t="s">
+        <v>2725</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1805" t="s">
+        <v>2728</v>
+      </c>
+      <c r="B1805" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1805" t="s">
+        <v>2726</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1806" s="5" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B1806" t="s">
+        <v>1895</v>
+      </c>
+      <c r="C1806" t="s">
+        <v>2732</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1807" s="5" t="s">
+        <v>2729</v>
+      </c>
+      <c r="B1807" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C1807" t="s">
+        <v>2730</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:C1677">
     <sortCondition ref="B1:B1677"/>

</xml_diff>